<commit_message>
Wait commands and Extent Reports
</commit_message>
<xml_diff>
--- a/GroceryApplication/src/test/resources/MainProjectTestData.xlsx
+++ b/GroceryApplication/src/test/resources/MainProjectTestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himaa\git\GroceryApplication\GroceryApplication\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3682A9-AF1F-454B-AFEB-22DB70979FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0AA3C04-D7B1-410E-9D3E-C1923A51044E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="NewsSearch" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>UserName</t>
   </si>
@@ -44,28 +45,34 @@
     <t>InvalidPwd</t>
   </si>
   <si>
-    <t>New news creation</t>
-  </si>
-  <si>
-    <t>Demo Project</t>
-  </si>
-  <si>
-    <t>libero non modi minus sunt.</t>
-  </si>
-  <si>
-    <t>non modi minus sunt.</t>
-  </si>
-  <si>
-    <t>Excepturi libero non modi minus sunt.</t>
-  </si>
-  <si>
-    <t>modi minus sunt.</t>
-  </si>
-  <si>
-    <t>content</t>
-  </si>
-  <si>
     <t>NewsContent</t>
+  </si>
+  <si>
+    <t>Expanded 6th generation interface</t>
+  </si>
+  <si>
+    <t>Multi-lateral multi-tasking instruction set</t>
+  </si>
+  <si>
+    <t>Assimilated impactful knowledge base</t>
+  </si>
+  <si>
+    <t>verna.johnson</t>
+  </si>
+  <si>
+    <t>barry.brekke</t>
+  </si>
+  <si>
+    <t>ocie.larson</t>
+  </si>
+  <si>
+    <t>ari.jaskolski</t>
+  </si>
+  <si>
+    <t>erik.hauck</t>
+  </si>
+  <si>
+    <t>oma.gulgowski</t>
   </si>
 </sst>
 </file>
@@ -93,10 +100,12 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF212529"/>
-      <name val="Aptos"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -137,20 +146,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,7 +447,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -488,10 +503,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A8E784-65EC-4251-B5F4-E8E955612260}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A8" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -499,77 +514,64 @@
     <col min="1" max="1" width="39.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" s="2"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -580,41 +582,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22FDE048-5BDA-4B17-B01A-F68EC54CE72B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.6328125" customWidth="1"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="38.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="B4" s="2"/>
     </row>

</xml_diff>